<commit_message>
Added Shawn's answers to mine and Fredy's.
</commit_message>
<xml_diff>
--- a/priorities/axe_rules.xlsx
+++ b/priorities/axe_rules.xlsx
@@ -14,6 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="impact">[1]Definitions!$A$2:$A$5</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="427">
   <si>
     <t>url</t>
   </si>
@@ -1379,6 +1385,42 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="data"/>
+      <sheetName val="Definitions"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Critical</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Serious</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Moderate</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Minor</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1681,7 +1723,7 @@
   <dimension ref="A1:H170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E84" sqref="E84:E170"/>
@@ -3366,6 +3408,9 @@
       <c r="D84" t="s">
         <v>169</v>
       </c>
+      <c r="E84" t="s">
+        <v>169</v>
+      </c>
       <c r="F84" t="s">
         <v>169</v>
       </c>
@@ -3389,6 +3434,9 @@
       <c r="D85" t="s">
         <v>169</v>
       </c>
+      <c r="E85" t="s">
+        <v>170</v>
+      </c>
       <c r="F85" t="s">
         <v>169</v>
       </c>
@@ -3411,6 +3459,9 @@
       </c>
       <c r="D86" t="s">
         <v>171</v>
+      </c>
+      <c r="E86" t="s">
+        <v>169</v>
       </c>
       <c r="F86" t="s">
         <v>169</v>
@@ -3432,6 +3483,9 @@
       <c r="D87" t="s">
         <v>171</v>
       </c>
+      <c r="E87" t="s">
+        <v>169</v>
+      </c>
       <c r="F87" t="s">
         <v>169</v>
       </c>
@@ -3452,6 +3506,9 @@
       <c r="D88" t="s">
         <v>171</v>
       </c>
+      <c r="E88" t="s">
+        <v>169</v>
+      </c>
       <c r="F88" t="s">
         <v>169</v>
       </c>
@@ -3472,6 +3529,9 @@
       <c r="D89" t="s">
         <v>169</v>
       </c>
+      <c r="E89" t="s">
+        <v>170</v>
+      </c>
       <c r="F89" t="s">
         <v>169</v>
       </c>
@@ -3492,6 +3552,9 @@
       <c r="D90" t="s">
         <v>171</v>
       </c>
+      <c r="E90" t="s">
+        <v>171</v>
+      </c>
       <c r="F90" t="s">
         <v>169</v>
       </c>
@@ -3513,6 +3576,9 @@
         <v>263</v>
       </c>
       <c r="D91" t="s">
+        <v>169</v>
+      </c>
+      <c r="E91" t="s">
         <v>169</v>
       </c>
       <c r="F91" t="s">
@@ -3535,6 +3601,9 @@
       <c r="D92" t="s">
         <v>171</v>
       </c>
+      <c r="E92" t="s">
+        <v>169</v>
+      </c>
       <c r="F92" t="s">
         <v>169</v>
       </c>
@@ -3558,6 +3627,9 @@
       <c r="D93" t="s">
         <v>171</v>
       </c>
+      <c r="E93" t="s">
+        <v>169</v>
+      </c>
       <c r="F93" t="s">
         <v>169</v>
       </c>
@@ -3581,6 +3653,9 @@
       <c r="D94" t="s">
         <v>170</v>
       </c>
+      <c r="E94" t="s">
+        <v>170</v>
+      </c>
       <c r="F94" t="s">
         <v>169</v>
       </c>
@@ -3603,6 +3678,9 @@
       </c>
       <c r="D95" t="s">
         <v>171</v>
+      </c>
+      <c r="E95" t="s">
+        <v>169</v>
       </c>
       <c r="F95" t="s">
         <v>169</v>
@@ -3624,6 +3702,9 @@
       <c r="D96" t="s">
         <v>171</v>
       </c>
+      <c r="E96" t="s">
+        <v>170</v>
+      </c>
       <c r="F96" t="s">
         <v>169</v>
       </c>
@@ -3647,6 +3728,9 @@
       <c r="D97" t="s">
         <v>170</v>
       </c>
+      <c r="E97" t="s">
+        <v>169</v>
+      </c>
       <c r="F97" t="s">
         <v>169</v>
       </c>
@@ -3670,6 +3754,9 @@
       <c r="D98" t="s">
         <v>170</v>
       </c>
+      <c r="E98" t="s">
+        <v>170</v>
+      </c>
       <c r="F98" t="s">
         <v>169</v>
       </c>
@@ -3693,6 +3780,9 @@
       <c r="D99" t="s">
         <v>169</v>
       </c>
+      <c r="E99" t="s">
+        <v>169</v>
+      </c>
       <c r="F99" t="s">
         <v>169</v>
       </c>
@@ -3714,6 +3804,9 @@
         <v>266</v>
       </c>
       <c r="D100" t="s">
+        <v>170</v>
+      </c>
+      <c r="E100" t="s">
         <v>170</v>
       </c>
       <c r="F100" t="s">
@@ -3736,6 +3829,9 @@
       <c r="D101" t="s">
         <v>170</v>
       </c>
+      <c r="E101" t="s">
+        <v>170</v>
+      </c>
       <c r="F101" t="s">
         <v>169</v>
       </c>
@@ -3759,6 +3855,9 @@
       <c r="D102" t="s">
         <v>169</v>
       </c>
+      <c r="E102" t="s">
+        <v>185</v>
+      </c>
       <c r="F102" t="s">
         <v>169</v>
       </c>
@@ -3782,6 +3881,9 @@
       <c r="D103" t="s">
         <v>169</v>
       </c>
+      <c r="E103" t="s">
+        <v>169</v>
+      </c>
       <c r="F103" t="s">
         <v>169</v>
       </c>
@@ -3803,6 +3905,9 @@
         <v>283</v>
       </c>
       <c r="D104" t="s">
+        <v>169</v>
+      </c>
+      <c r="E104" t="s">
         <v>169</v>
       </c>
       <c r="F104" t="s">
@@ -3825,6 +3930,9 @@
       <c r="D105" t="s">
         <v>169</v>
       </c>
+      <c r="E105" t="s">
+        <v>171</v>
+      </c>
       <c r="F105" t="s">
         <v>171</v>
       </c>
@@ -3848,6 +3956,9 @@
       <c r="D106" t="s">
         <v>169</v>
       </c>
+      <c r="E106" t="s">
+        <v>169</v>
+      </c>
       <c r="F106" t="s">
         <v>171</v>
       </c>
@@ -3871,6 +3982,9 @@
       <c r="D107" t="s">
         <v>185</v>
       </c>
+      <c r="E107" t="s">
+        <v>185</v>
+      </c>
       <c r="F107" t="s">
         <v>169</v>
       </c>
@@ -3892,6 +4006,9 @@
         <v>270</v>
       </c>
       <c r="D108" t="s">
+        <v>185</v>
+      </c>
+      <c r="E108" t="s">
         <v>185</v>
       </c>
       <c r="F108" t="s">
@@ -3914,6 +4031,9 @@
       <c r="D109" t="s">
         <v>171</v>
       </c>
+      <c r="E109" t="s">
+        <v>169</v>
+      </c>
       <c r="F109" t="s">
         <v>169</v>
       </c>
@@ -3934,6 +4054,9 @@
       <c r="D110" t="s">
         <v>171</v>
       </c>
+      <c r="E110" t="s">
+        <v>169</v>
+      </c>
       <c r="F110" t="s">
         <v>169</v>
       </c>
@@ -3957,6 +4080,9 @@
       <c r="D111" t="s">
         <v>171</v>
       </c>
+      <c r="E111" t="s">
+        <v>169</v>
+      </c>
       <c r="F111" t="s">
         <v>169</v>
       </c>
@@ -3980,6 +4106,9 @@
       <c r="D112" t="s">
         <v>169</v>
       </c>
+      <c r="E112" t="s">
+        <v>170</v>
+      </c>
       <c r="F112" t="s">
         <v>169</v>
       </c>
@@ -4003,6 +4132,9 @@
       <c r="D113" t="s">
         <v>169</v>
       </c>
+      <c r="E113" t="s">
+        <v>170</v>
+      </c>
       <c r="F113" t="s">
         <v>169</v>
       </c>
@@ -4024,6 +4156,9 @@
         <v>288</v>
       </c>
       <c r="D114" t="s">
+        <v>169</v>
+      </c>
+      <c r="E114" t="s">
         <v>169</v>
       </c>
       <c r="F114" t="s">
@@ -4046,6 +4181,9 @@
       <c r="D115" t="s">
         <v>171</v>
       </c>
+      <c r="E115" t="s">
+        <v>169</v>
+      </c>
       <c r="F115" t="s">
         <v>169</v>
       </c>
@@ -4067,6 +4205,9 @@
         <v>290</v>
       </c>
       <c r="D116" t="s">
+        <v>169</v>
+      </c>
+      <c r="E116" t="s">
         <v>169</v>
       </c>
       <c r="F116" t="s">
@@ -4089,6 +4230,9 @@
       <c r="D117" t="s">
         <v>171</v>
       </c>
+      <c r="E117" t="s">
+        <v>169</v>
+      </c>
       <c r="F117" t="s">
         <v>169</v>
       </c>
@@ -4109,6 +4253,9 @@
       <c r="D118" t="s">
         <v>171</v>
       </c>
+      <c r="E118" t="s">
+        <v>169</v>
+      </c>
       <c r="F118" t="s">
         <v>169</v>
       </c>
@@ -4129,6 +4276,9 @@
       <c r="D119" t="s">
         <v>169</v>
       </c>
+      <c r="E119" t="s">
+        <v>170</v>
+      </c>
       <c r="F119" t="s">
         <v>169</v>
       </c>
@@ -4152,6 +4302,9 @@
       <c r="D120" t="s">
         <v>171</v>
       </c>
+      <c r="E120" t="s">
+        <v>171</v>
+      </c>
       <c r="F120" t="s">
         <v>169</v>
       </c>
@@ -4175,6 +4328,9 @@
       <c r="D121" t="s">
         <v>171</v>
       </c>
+      <c r="E121" t="s">
+        <v>169</v>
+      </c>
       <c r="F121" t="s">
         <v>169</v>
       </c>
@@ -4198,6 +4354,9 @@
       <c r="D122" t="s">
         <v>171</v>
       </c>
+      <c r="E122" t="s">
+        <v>169</v>
+      </c>
       <c r="F122" t="s">
         <v>169</v>
       </c>
@@ -4221,6 +4380,9 @@
       <c r="D123" t="s">
         <v>169</v>
       </c>
+      <c r="E123" t="s">
+        <v>170</v>
+      </c>
       <c r="F123" t="s">
         <v>169</v>
       </c>
@@ -4244,6 +4406,9 @@
       <c r="D124" t="s">
         <v>170</v>
       </c>
+      <c r="E124" t="s">
+        <v>170</v>
+      </c>
       <c r="F124" t="s">
         <v>169</v>
       </c>
@@ -4266,6 +4431,9 @@
       </c>
       <c r="D125" t="s">
         <v>169</v>
+      </c>
+      <c r="E125" t="s">
+        <v>170</v>
       </c>
       <c r="F125" t="s">
         <v>169</v>
@@ -4287,6 +4455,9 @@
       <c r="D126" t="s">
         <v>170</v>
       </c>
+      <c r="E126" t="s">
+        <v>170</v>
+      </c>
       <c r="F126" t="s">
         <v>169</v>
       </c>
@@ -4310,6 +4481,9 @@
       <c r="D127" t="s">
         <v>169</v>
       </c>
+      <c r="E127" t="s">
+        <v>169</v>
+      </c>
       <c r="F127" t="s">
         <v>169</v>
       </c>
@@ -4333,6 +4507,9 @@
       <c r="D128" t="s">
         <v>171</v>
       </c>
+      <c r="E128" t="s">
+        <v>169</v>
+      </c>
       <c r="F128" t="s">
         <v>169</v>
       </c>
@@ -4356,6 +4533,9 @@
       <c r="D129" t="s">
         <v>169</v>
       </c>
+      <c r="E129" t="s">
+        <v>170</v>
+      </c>
       <c r="F129" t="s">
         <v>169</v>
       </c>
@@ -4377,6 +4557,9 @@
         <v>369</v>
       </c>
       <c r="D130" t="s">
+        <v>185</v>
+      </c>
+      <c r="E130" t="s">
         <v>185</v>
       </c>
       <c r="F130" t="s">
@@ -4399,6 +4582,9 @@
       <c r="D131" t="s">
         <v>169</v>
       </c>
+      <c r="E131" t="s">
+        <v>170</v>
+      </c>
       <c r="F131" t="s">
         <v>169</v>
       </c>
@@ -4419,6 +4605,9 @@
       <c r="D132" t="s">
         <v>170</v>
       </c>
+      <c r="E132" t="s">
+        <v>171</v>
+      </c>
       <c r="F132" t="s">
         <v>169</v>
       </c>
@@ -4440,6 +4629,9 @@
         <v>309</v>
       </c>
       <c r="D133" t="s">
+        <v>169</v>
+      </c>
+      <c r="E133" t="s">
         <v>169</v>
       </c>
       <c r="F133" t="s">
@@ -4462,6 +4654,9 @@
       <c r="D134" t="s">
         <v>171</v>
       </c>
+      <c r="E134" t="s">
+        <v>169</v>
+      </c>
       <c r="F134" t="s">
         <v>169</v>
       </c>
@@ -4485,6 +4680,9 @@
       <c r="D135" t="s">
         <v>171</v>
       </c>
+      <c r="E135" t="s">
+        <v>169</v>
+      </c>
       <c r="F135" t="s">
         <v>169</v>
       </c>
@@ -4508,6 +4706,9 @@
       <c r="D136" t="s">
         <v>169</v>
       </c>
+      <c r="E136" t="s">
+        <v>170</v>
+      </c>
       <c r="F136" t="s">
         <v>169</v>
       </c>
@@ -4529,6 +4730,9 @@
         <v>324</v>
       </c>
       <c r="D137" t="s">
+        <v>169</v>
+      </c>
+      <c r="E137" t="s">
         <v>169</v>
       </c>
       <c r="F137" t="s">
@@ -4551,6 +4755,9 @@
       <c r="D138" t="s">
         <v>169</v>
       </c>
+      <c r="E138" t="s">
+        <v>169</v>
+      </c>
       <c r="F138" t="s">
         <v>169</v>
       </c>
@@ -4573,6 +4780,9 @@
       </c>
       <c r="D139" t="s">
         <v>171</v>
+      </c>
+      <c r="E139" t="s">
+        <v>170</v>
       </c>
       <c r="F139" t="s">
         <v>169</v>
@@ -4594,6 +4804,9 @@
       <c r="D140" t="s">
         <v>169</v>
       </c>
+      <c r="E140" t="s">
+        <v>169</v>
+      </c>
       <c r="F140" t="s">
         <v>169</v>
       </c>
@@ -4617,6 +4830,9 @@
       <c r="D141" t="s">
         <v>170</v>
       </c>
+      <c r="E141" t="s">
+        <v>169</v>
+      </c>
       <c r="F141" t="s">
         <v>169</v>
       </c>
@@ -4640,6 +4856,9 @@
       <c r="D142" t="s">
         <v>171</v>
       </c>
+      <c r="E142" t="s">
+        <v>170</v>
+      </c>
       <c r="F142" t="s">
         <v>169</v>
       </c>
@@ -4663,6 +4882,9 @@
       <c r="D143" t="s">
         <v>169</v>
       </c>
+      <c r="E143" t="s">
+        <v>170</v>
+      </c>
       <c r="F143" t="s">
         <v>169</v>
       </c>
@@ -4686,6 +4908,9 @@
       <c r="D144" t="s">
         <v>171</v>
       </c>
+      <c r="E144" t="s">
+        <v>169</v>
+      </c>
       <c r="F144" t="s">
         <v>169</v>
       </c>
@@ -4709,6 +4934,9 @@
       <c r="D145" t="s">
         <v>171</v>
       </c>
+      <c r="E145" t="s">
+        <v>169</v>
+      </c>
       <c r="F145" t="s">
         <v>169</v>
       </c>
@@ -4732,6 +4960,9 @@
       <c r="D146" t="s">
         <v>170</v>
       </c>
+      <c r="E146" t="s">
+        <v>170</v>
+      </c>
       <c r="F146" t="s">
         <v>169</v>
       </c>
@@ -4755,6 +4986,9 @@
       <c r="D147" t="s">
         <v>171</v>
       </c>
+      <c r="E147" t="s">
+        <v>169</v>
+      </c>
       <c r="F147" t="s">
         <v>169</v>
       </c>
@@ -4778,6 +5012,9 @@
       <c r="D148" t="s">
         <v>171</v>
       </c>
+      <c r="E148" t="s">
+        <v>169</v>
+      </c>
       <c r="F148" t="s">
         <v>170</v>
       </c>
@@ -4801,6 +5038,9 @@
       <c r="D149" t="s">
         <v>171</v>
       </c>
+      <c r="E149" t="s">
+        <v>169</v>
+      </c>
       <c r="F149" t="s">
         <v>170</v>
       </c>
@@ -4824,6 +5064,9 @@
       <c r="D150" t="s">
         <v>169</v>
       </c>
+      <c r="E150" t="s">
+        <v>171</v>
+      </c>
       <c r="F150" t="s">
         <v>170</v>
       </c>
@@ -4847,6 +5090,9 @@
       <c r="D151" t="s">
         <v>171</v>
       </c>
+      <c r="E151" t="s">
+        <v>171</v>
+      </c>
       <c r="F151" t="s">
         <v>169</v>
       </c>
@@ -4869,6 +5115,9 @@
       </c>
       <c r="D152" t="s">
         <v>185</v>
+      </c>
+      <c r="E152" t="s">
+        <v>170</v>
       </c>
       <c r="F152" t="s">
         <v>169</v>
@@ -4890,6 +5139,9 @@
       <c r="D153" t="s">
         <v>171</v>
       </c>
+      <c r="E153" t="s">
+        <v>171</v>
+      </c>
       <c r="F153" t="s">
         <v>169</v>
       </c>
@@ -4912,6 +5164,9 @@
       </c>
       <c r="D154" t="s">
         <v>170</v>
+      </c>
+      <c r="E154" t="s">
+        <v>169</v>
       </c>
       <c r="F154" t="s">
         <v>169</v>
@@ -4933,6 +5188,9 @@
       <c r="D155" t="s">
         <v>171</v>
       </c>
+      <c r="E155" t="s">
+        <v>170</v>
+      </c>
       <c r="F155" t="s">
         <v>171</v>
       </c>
@@ -4951,6 +5209,9 @@
         <v>229</v>
       </c>
       <c r="D156" t="s">
+        <v>169</v>
+      </c>
+      <c r="E156" t="s">
         <v>169</v>
       </c>
       <c r="F156" t="s">
@@ -4990,6 +5251,9 @@
       <c r="D158" t="s">
         <v>169</v>
       </c>
+      <c r="E158" t="s">
+        <v>170</v>
+      </c>
       <c r="F158" t="s">
         <v>169</v>
       </c>
@@ -5007,6 +5271,9 @@
       <c r="D159" t="s">
         <v>169</v>
       </c>
+      <c r="E159" t="s">
+        <v>169</v>
+      </c>
       <c r="F159" t="s">
         <v>169</v>
       </c>
@@ -5024,6 +5291,9 @@
       <c r="D160" t="s">
         <v>169</v>
       </c>
+      <c r="E160" t="s">
+        <v>169</v>
+      </c>
       <c r="F160" t="s">
         <v>169</v>
       </c>
@@ -5041,6 +5311,9 @@
       <c r="D161" t="s">
         <v>171</v>
       </c>
+      <c r="E161" t="s">
+        <v>169</v>
+      </c>
       <c r="F161" t="s">
         <v>169</v>
       </c>
@@ -5095,6 +5368,9 @@
       <c r="D164" t="s">
         <v>170</v>
       </c>
+      <c r="E164" t="s">
+        <v>169</v>
+      </c>
       <c r="F164" t="s">
         <v>169</v>
       </c>
@@ -5114,6 +5390,9 @@
       </c>
       <c r="D165" t="s">
         <v>170</v>
+      </c>
+      <c r="E165" t="s">
+        <v>169</v>
       </c>
       <c r="F165" t="s">
         <v>169</v>
@@ -5132,6 +5411,9 @@
       <c r="D166" t="s">
         <v>171</v>
       </c>
+      <c r="E166" t="s">
+        <v>169</v>
+      </c>
       <c r="F166" t="s">
         <v>169</v>
       </c>
@@ -5149,6 +5431,9 @@
       <c r="D167" t="s">
         <v>171</v>
       </c>
+      <c r="E167" t="s">
+        <v>169</v>
+      </c>
       <c r="F167" t="s">
         <v>169</v>
       </c>
@@ -5166,6 +5451,9 @@
       <c r="D168" t="s">
         <v>171</v>
       </c>
+      <c r="E168" t="s">
+        <v>169</v>
+      </c>
       <c r="F168" t="s">
         <v>169</v>
       </c>
@@ -5186,6 +5474,9 @@
       <c r="D169" t="s">
         <v>170</v>
       </c>
+      <c r="E169" t="s">
+        <v>170</v>
+      </c>
       <c r="F169" t="s">
         <v>169</v>
       </c>
@@ -5206,6 +5497,9 @@
       <c r="D170" t="s">
         <v>170</v>
       </c>
+      <c r="E170" t="s">
+        <v>169</v>
+      </c>
       <c r="F170" t="s">
         <v>169</v>
       </c>
@@ -5217,6 +5511,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84:E170">
+      <formula1>impact</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="C111" r:id="rId1"/>
     <hyperlink ref="C90" r:id="rId2"/>

</xml_diff>